<commit_message>
Aanpassingen notatie product backlog + aanmaak presentatie Sprint review 0
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Desktop\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8467452-C611-46DB-8304-A440AC799926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5FAAB0-1E55-4CE1-9825-8C5C5B39AC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>1. Interface van zichtbare sensordata</t>
   </si>
   <si>
-    <t>Ik wil duidelijk kunnen zien in welke hoek de boerderij zich bevindt en in welke toestand de andere onderdelen verkeren.</t>
-  </si>
-  <si>
     <t>2. Hoekberekening met behulp van sensoren</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>4. Werkend schaalmodel</t>
-  </si>
-  <si>
-    <t>Ik wil graag een duidelijk en werkend schaalmodel zien, waarin goed wordt weergegeven wat er gebeurt wanneer de boerderij uit balans raakt</t>
   </si>
   <si>
     <t>1. Sensordata uitlezen en verwerken
@@ -114,9 +108,6 @@
 De sensor  data moet gebruikt kunnen worden de het stabilzatie algoritme</t>
   </si>
   <si>
-    <t>5. Algoritme om floating farm water pass houden</t>
-  </si>
-  <si>
     <t>De pompen brengen water in een uit de hier voor bestemde ruimtes</t>
   </si>
   <si>
@@ -136,15 +127,6 @@
   </si>
   <si>
     <t>verbetetingen product backlog</t>
-  </si>
-  <si>
-    <t>Als systeem wil ik de hoek nauwkeurig berekenen, zodat ik weet naar welke kant water verplaatst moet worden</t>
-  </si>
-  <si>
-    <t>Als beheerder wil ik dat de boerderij zichzelf stabiliseert door water te verplaatsen met pompen, zodat dit duurzaam gebeurt.</t>
-  </si>
-  <si>
-    <t>Als systeem wil ik sensordata omzetten in pompacties, zodat het platform automatisch waterpas blijft.</t>
   </si>
   <si>
     <t>1. Onderzoek naar data-analyse en filtering
@@ -157,6 +139,24 @@
 3. Testplant uitvoeren en  de beste plaatsing van de motoren keizen
 4. Pompen implementeren in het schaalmodel
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als beheerder wil ik dat de boerderij zichzelf stabiliseert door water te verplaatsen met pompen, zodat dit duurzaam en efficient gebeurd. </t>
+  </si>
+  <si>
+    <t>Als systeem wil ik de hoek nauwkeurig berekenen, zodat ik weet naar welke kant water verplaatst moet worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik wil duidelijk kunnen zien in welke hoek de boerderij zich bevindt en in welke toestand de andere onderdelen verkeren, om een duidelijk overzicht te hebben van het systeem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik wil graag een duidelijk en werkend schaalmodel zien, waarin goed wordt weergegeven wat er gebeurt wanneer de boerderij uit balans raakt. </t>
+  </si>
+  <si>
+    <t>5. Algoritme om floating farm waterpas houden</t>
+  </si>
+  <si>
+    <t>Als systeem wil ik sensordata waterpas hebben, zodat ik altijd nauwkeurige en realistische lezingen krijg.</t>
   </si>
 </sst>
 </file>
@@ -233,7 +233,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -251,7 +251,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1417,21 +1417,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="51.5546875" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.90625" customWidth="1"/>
+    <col min="3" max="3" width="51.54296875" customWidth="1"/>
+    <col min="4" max="4" width="38.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1457,95 +1459,95 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1553,7 +1555,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1561,7 +1563,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1569,7 +1571,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1577,7 +1579,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1585,7 +1587,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1593,7 +1595,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1609,7 +1611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1649,34 +1651,34 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aanpassingen sprint presentatie + product backlog
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5FAAB0-1E55-4CE1-9825-8C5C5B39AC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0623BE-C9B0-4E6B-A405-444D9AE4F433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>De pompen brengen water in een uit de hier voor bestemde ruimtes</t>
   </si>
   <si>
-    <t xml:space="preserve">Het algortime stuurd de pompen aan op basis van de sensor data. En deze zo aanstuurd dat het platform  waterpass wordt </t>
-  </si>
-  <si>
     <t>Het schaal model is functoneel representief van de floating farm. Hier op kunnen wij ons idee testen/presenteren</t>
   </si>
   <si>
@@ -127,11 +124,6 @@
   </si>
   <si>
     <t>verbetetingen product backlog</t>
-  </si>
-  <si>
-    <t>1. Onderzoek naar data-analyse en filtering
-2. Algoratime om sensor data om te zetten in acties voor pompen
-3. Algoritme testen en kalibreren</t>
   </si>
   <si>
     <t xml:space="preserve">1. Geschikte pomp uitzoeken
@@ -153,10 +145,18 @@
     <t xml:space="preserve">Ik wil graag een duidelijk en werkend schaalmodel zien, waarin goed wordt weergegeven wat er gebeurt wanneer de boerderij uit balans raakt. </t>
   </si>
   <si>
-    <t>5. Algoritme om floating farm waterpas houden</t>
-  </si>
-  <si>
     <t>Als systeem wil ik sensordata waterpas hebben, zodat ik altijd nauwkeurige en realistische lezingen krijg.</t>
+  </si>
+  <si>
+    <t>1. Onderzoek naar data-analyse en filtering
+2. Algoritme om sensor data waterpas te houden
+3. Algoritme testen en kalibreren</t>
+  </si>
+  <si>
+    <t>Het algortime geeft accurate data die waterpas is en gehouden word.</t>
+  </si>
+  <si>
+    <t>5. Algoritme om constante data over de positie van de Floating Farm te krijgen</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1464,7 +1464,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
@@ -1480,7 +1480,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -1498,10 +1498,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -1516,31 +1516,31 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
@@ -1548,10 +1548,6 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
     </row>
@@ -1659,10 +1655,10 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -1670,7 +1666,7 @@
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -1678,7 +1674,7 @@
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Meer aanpassingen product backlog
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0623BE-C9B0-4E6B-A405-444D9AE4F433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9AB4C0-9D71-4CE3-831A-7D630726D0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Requirement</t>
   </si>
@@ -108,9 +108,6 @@
 De sensor  data moet gebruikt kunnen worden de het stabilzatie algoritme</t>
   </si>
   <si>
-    <t>De pompen brengen water in een uit de hier voor bestemde ruimtes</t>
-  </si>
-  <si>
     <t>Het schaal model is functoneel representief van de floating farm. Hier op kunnen wij ons idee testen/presenteren</t>
   </si>
   <si>
@@ -124,13 +121,6 @@
   </si>
   <si>
     <t>verbetetingen product backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Geschikte pomp uitzoeken
-2. Testplan opstellen
-3. Testplant uitvoeren en  de beste plaatsing van de motoren keizen
-4. Pompen implementeren in het schaalmodel
-</t>
   </si>
   <si>
     <t xml:space="preserve">Als beheerder wil ik dat de boerderij zichzelf stabiliseert door water te verplaatsen met pompen, zodat dit duurzaam en efficient gebeurd. </t>
@@ -157,6 +147,30 @@
   </si>
   <si>
     <t>5. Algoritme om constante data over de positie van de Floating Farm te krijgen</t>
+  </si>
+  <si>
+    <t>De pompen brengen water in een uit de hier voor bestemde ruimtes.</t>
+  </si>
+  <si>
+    <t>1. Geschikte pomp uitzoeken
+2. Testen en de beste plaatsing van de pompen kiezen
+3. Pompen implementeren in het schaalmodel</t>
+  </si>
+  <si>
+    <t>6. Algoritme om de pompen aan te sturen op basis van sensordata.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als systeemeigenaar wil ik dat het systeem uit zichzelf de boerderij stabiliseert op basis van de gemeten data, zodat deze niet door een mens geregeld hoeft te worden en altijd nauwkeurig zal zijn. </t>
+  </si>
+  <si>
+    <t>1. Testen gebruik van pompen + sensor(en)
+2. Implementeren en tunen tot gewenst gebruik</t>
+  </si>
+  <si>
+    <t>De pompen worden automatisch aangestuurd door het algoritme op basis van de sensordata</t>
+  </si>
+  <si>
+    <t>Een interface met bruikbare en relevante data die door iedereen gebruikt, bediend en bekeken kan worden</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1464,12 +1478,14 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1480,7 +1496,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -1493,18 +1509,18 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -1516,13 +1532,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -1531,24 +1547,38 @@
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E7" s="2"/>
+    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1655,10 +1685,10 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -1666,7 +1696,7 @@
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -1674,7 +1704,7 @@
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aanpassingen backlog en presentatie :P
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9AB4C0-9D71-4CE3-831A-7D630726D0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C502DE-2C9C-4977-AA13-4E52103462B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -95,12 +95,6 @@
 4. Test uitvoeren waarbij onbalans en stabilisatie zichtbaar worden</t>
   </si>
   <si>
-    <t>1. Geschikte sensoren uitzoeken
-2. testplan opstellen 
-3. testplan uitvoeren en sensor kiezen
-4. sensor kalibreren</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -171,6 +165,11 @@
   </si>
   <si>
     <t>Een interface met bruikbare en relevante data die door iedereen gebruikt, bediend en bekeken kan worden</t>
+  </si>
+  <si>
+    <t>1. Geschikte sensoren uitzoeken
+2. Sensoren testen en kiezen
+3. sensor kalibreren</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1478,16 +1477,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -1496,16 +1495,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -1514,16 +1513,16 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -1532,52 +1531,52 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1685,10 +1684,10 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -1696,7 +1695,7 @@
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -1704,7 +1703,7 @@
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aanpassing ballasttank onderzoek + product backlog
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BD695C-939F-4682-B2C2-2B19BDCDBDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331376A2-EBEB-444B-8DA4-C0772A31B419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -78,15 +78,7 @@
     <t>2. Hoekberekening met behulp van sensoren</t>
   </si>
   <si>
-    <t>3. Stabiliseren met waterpompen</t>
-  </si>
-  <si>
     <t>4. Werkend schaalmodel</t>
-  </si>
-  <si>
-    <t>1. Sensordata uitlezen en verwerken
-2. Data versturen naar webserver
-3. Data overzichtelijk weergeven in een interface</t>
   </si>
   <si>
     <t>1. schaal 3D-model ontwerpen
@@ -140,14 +132,6 @@
     <t>Het algortime geeft accurate data die waterpas is en gehouden word.</t>
   </si>
   <si>
-    <t>De pompen brengen water in een uit de hier voor bestemde ruimtes.</t>
-  </si>
-  <si>
-    <t>1. Geschikte pomp uitzoeken
-2. Testen en de beste plaatsing van de pompen kiezen
-3. Pompen implementeren in het schaalmodel</t>
-  </si>
-  <si>
     <t>6. Algoritme om de pompen aan te sturen op basis van sensordata.</t>
   </si>
   <si>
@@ -170,6 +154,22 @@
   </si>
   <si>
     <t>5. Algoritme om constante en nauwkeurige data op te halen van de sensor</t>
+  </si>
+  <si>
+    <t>3. Stabiliseren met waterpompsysteem</t>
+  </si>
+  <si>
+    <t>1. Geschikte pompsystemen uitzoeken
+2. Testen en de beste plaatsing van de bijbehorende pompen kiezen
+3. Pompsysteem implementeren in het schaalmodel</t>
+  </si>
+  <si>
+    <t>Het pompsysteem brengt water in en uit de hier voor bestemde ruimtes om de Floating Farm te stabiliseren.</t>
+  </si>
+  <si>
+    <t>1. Sensordata uitlezen en verwerken
+2. Data versturen naar een interface
+3. Data overzichtelijk en netjesweergeven in een interface</t>
   </si>
 </sst>
 </file>
@@ -201,18 +201,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,13 +231,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1431,7 +1425,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1473,20 +1467,20 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -1495,88 +1489,88 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -1684,26 +1678,26 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Requirementspecificatie toegevoegd + product backlog uitgebreid
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416F598-D2F7-4CFD-B4E9-2416A9F9E118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4569AE77-DDDB-4D4C-9605-D8F440D3CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Requirement</t>
   </si>
@@ -70,15 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">Totaal: </t>
-  </si>
-  <si>
-    <t>1. Interface van zichtbare sensordata</t>
-  </si>
-  <si>
-    <t>2. Hoekberekening met behulp van sensoren</t>
-  </si>
-  <si>
-    <t>4. Werkend schaalmodel</t>
   </si>
   <si>
     <t>1. schaal 3D-model ontwerpen
@@ -132,9 +123,6 @@
     <t>Het algortime geeft accurate data die waterpas is en gehouden word.</t>
   </si>
   <si>
-    <t>6. Algoritme om de pompen aan te sturen op basis van sensordata.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Als systeemeigenaar wil ik dat het systeem uit zichzelf de boerderij stabiliseert op basis van de gemeten data, zodat deze niet door een mens geregeld hoeft te worden en altijd nauwkeurig zal zijn. </t>
   </si>
   <si>
@@ -153,12 +141,6 @@
 3. sensor kalibreren</t>
   </si>
   <si>
-    <t>5. Algoritme om constante en nauwkeurige data op te halen van de sensor</t>
-  </si>
-  <si>
-    <t>3. Stabiliseren met waterpompsysteem</t>
-  </si>
-  <si>
     <t>1. Geschikte pompsystemen uitzoeken
 2. Testen en de beste plaatsing van de bijbehorende pompen kiezen
 3. Pompsysteem implementeren in het schaalmodel</t>
@@ -172,18 +154,6 @@
 3. Data weergeven op een interface</t>
   </si>
   <si>
-    <t>7. De interface heeft…</t>
-  </si>
-  <si>
-    <t>Als gebruiker wil ik dat … zodat …</t>
-  </si>
-  <si>
-    <t>De interface bevat</t>
-  </si>
-  <si>
-    <t>8. Het schaalmodel is qua uiterlijk realistisch</t>
-  </si>
-  <si>
     <t xml:space="preserve">Als opdrachtgever wil ik dat het schaalmodel en realistische representatie is van het echte gebouw, zodat het compleet duidelijk is hoe het uiteindelijk in werking gaat. </t>
   </si>
   <si>
@@ -196,6 +166,46 @@
   </si>
   <si>
     <t>Het schaalmodel is op 1:100 schaal van de Floating Farm, met zo veel mogelijk detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Het systeem heeft een interface met sensordata in een 
+precieze grafiek. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Het systeem bepaalt de hoek van Floating Farm relatief tot waterpas met behulp van een sensor(en). </t>
+  </si>
+  <si>
+    <t>3. Het systeem kan de Floating Farm in de Rotterdamse Haven stabiliseren met een waterpompsysteem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Het eindproduct bevat een schaalmodel die zichtzelf waterpas houd met onze oplossing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Het systeem heeft een algoritme om met nauwkeurigheid en precisie constant data op kan halen van de MPU-6050. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Het systeem heeft een algoritme om de pompen aan te kunnen sturen met gebruik van de afgelezen sensordata bij de MPU-6050 vandaan. </t>
+  </si>
+  <si>
+    <t>8. Het schaalmodel lijkt sprekend op het fysieke uiterlijk van
+ de Floating Farm die in de Rotterdamse Haven ligt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. De miniatuur waterpompen kunnen binnen … minuten de ballasttanks opvullen en leeg laten lopen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. De Ballasttanks kunnen de Floating Farm … graden kantelen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Het complete systeem heeft een maximale afwijking 
+van … graden tot waterpas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Het systeem is bruikbaar voor toekomstige designs en 
+uitbreidingen aan de Floating Farm. </t>
+  </si>
+  <si>
+    <t>Als eigenaar wil ik dat de pompen de ballasttanks binnen … minuten kunnen legen en opvullen om in noodgevallen snel te kunnen reageren.</t>
   </si>
 </sst>
 </file>
@@ -247,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -258,9 +268,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1450,13 +1457,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.453125" customWidth="1"/>
+    <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="46.90625" customWidth="1"/>
     <col min="3" max="3" width="51.54296875" customWidth="1"/>
     <col min="4" max="4" width="38.08984375" customWidth="1"/>
@@ -1494,164 +1501,168 @@
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>43</v>
+      <c r="A9" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -1722,10 +1733,10 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -1733,7 +1744,7 @@
         <v>45916</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -1741,7 +1752,7 @@
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toevoeging document + product backlog uitgebreid
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4569AE77-DDDB-4D4C-9605-D8F440D3CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466BBB17-C94E-4A01-A38A-2AA82E2141AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Requirement</t>
   </si>
@@ -165,9 +165,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Het schaalmodel is op 1:100 schaal van de Floating Farm, met zo veel mogelijk detail</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Het systeem heeft een interface met sensordata in een 
 precieze grafiek. </t>
   </si>
@@ -206,6 +203,53 @@
   </si>
   <si>
     <t>Als eigenaar wil ik dat de pompen de ballasttanks binnen … minuten kunnen legen en opvullen om in noodgevallen snel te kunnen reageren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als eigenaar wil ik dat de Ballasttanks de Floating Farm … graden kunnen kantelen, zodat mijn boerderij altijd waterpas kan staan. </t>
+  </si>
+  <si>
+    <t>1. Berekenen hoeveel drijfvermogen de Ballasttanks moeten hebben.
+2. Maak de Ballasttanks gebaseerd op deze berekeningen.</t>
+  </si>
+  <si>
+    <t>1. Overleg met opdrachtgever binnen hoeveel minuten.
+2. Gebaseerd op het overleg berekenen hoeveel water de pompen moeten kunnen verplaatsen om dit te bereiken. 
+3. Pomp uitkiezen en bestellen
+4. Pomp implementeren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De pompen kunnen de ballasttanks binnen … minuten leeg en vol pompen/laten lopen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als eigenaar wil ik dat het systeem niet meer dan … graden afwijkt om te zorgen dat mijn lezingen nauwkeurig en correct zijn. </t>
+  </si>
+  <si>
+    <t>1. Maximale afwijking berekenen
+2.  Huidige afwijkingen bekijken
+3. Aanpassingen implementeren zo nodig</t>
+  </si>
+  <si>
+    <t>De ballasttanks hebben het drijfvermogen/inhoud om de Floating Farm … graden te draaien.</t>
+  </si>
+  <si>
+    <t>Het schaalmodel is op 1:100 schaal van de Floating Farm, met zo veel mogelijk detail.</t>
+  </si>
+  <si>
+    <t>Het systeem heeft ten alle tijden niet meer dan … graden afwijking tot waterpas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als eigenaar wil ik dat het design uitbreidbaar en herbruikbaar is, om te zorgen dat dit probleem opgelost is voordat het onstaat bij volgende Floating Farms. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Onderzoeken wat er nodig is om een design herbruikbaar te maken.
+2. Rekening houden met de onderzochte dingen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het systeem is gemakkelijk toe te passen bij
+ toekomstige Floating Farms en is ook makkelijk uitbreidbaar. </t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1501,7 +1545,7 @@
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>21</v>
@@ -1519,7 +1563,7 @@
     </row>
     <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -1537,7 +1581,7 @@
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -1555,7 +1599,7 @@
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
@@ -1573,7 +1617,7 @@
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -1591,7 +1635,7 @@
     </row>
     <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>26</v>
@@ -1607,15 +1651,19 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1623,7 +1671,7 @@
     </row>
     <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>34</v>
@@ -1632,41 +1680,65 @@
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Sprint 2 presentatie aangemaakt
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466BBB17-C94E-4A01-A38A-2AA82E2141AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A285AC4F-9ECD-41EA-B7FC-E6FFF8AB721F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>maak document en eerste versie backlog</t>
   </si>
   <si>
-    <t>verbetetingen product backlog</t>
-  </si>
-  <si>
     <t xml:space="preserve">Als beheerder wil ik dat de boerderij zichzelf stabiliseert door water te verplaatsen met pompen, zodat dit duurzaam en efficient gebeurd. </t>
   </si>
   <si>
@@ -163,10 +160,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Het systeem heeft een interface met sensordata in een 
-precieze grafiek. </t>
   </si>
   <si>
     <t xml:space="preserve">2. Het systeem bepaalt de hoek van Floating Farm relatief tot waterpas met behulp van een sensor(en). </t>
@@ -250,6 +243,12 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>verbeteringen product backlog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Het systeem heeft een interface met sensordata waarin de data overzichtelijk voor weergeven. Bijv. een grafiek.  </t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,16 +1544,16 @@
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -1563,13 +1562,13 @@
     </row>
     <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1581,16 +1580,16 @@
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>12</v>
@@ -1599,10 +1598,10 @@
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -1617,16 +1616,16 @@
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -1635,16 +1634,16 @@
     </row>
     <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>12</v>
@@ -1653,16 +1652,16 @@
     </row>
     <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
@@ -1671,34 +1670,34 @@
     </row>
     <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
@@ -1707,16 +1706,16 @@
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
@@ -1725,19 +1724,19 @@
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -1794,7 +1793,7 @@
   <dimension ref="B4:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1824,7 +1823,7 @@
         <v>45919</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update uitgaves en product backlog
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A074FC-EF8D-40D1-9DB0-51B7F25A9891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BE5902-D5E5-4F90-8708-1900D2EE78C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
@@ -1597,7 +1597,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Elektrisch Schema toegevoegd + 50% presentatie aangemaakt
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BE5902-D5E5-4F90-8708-1900D2EE78C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C58C162-6206-4A83-83E9-09DDD22CBDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
+    <workbookView xWindow="1770" yWindow="1100" windowWidth="19200" windowHeight="11170" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Opleverset folders aangepast + presentatie verebeterd
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E86AEBF-7CE3-45A0-89E3-1B1B423042A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F0AE52-DF62-418A-AC85-E3EAA42579DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Aanmaak sprint presentatie 5, aanpassing testplan
</commit_message>
<xml_diff>
--- a/Opleverset/Documentatie/Product backlog.xlsx
+++ b/Opleverset/Documentatie/Product backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Desktop\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrtha\Documents\GitHub\Project-5-6---Floating-Farm\Opleverset\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15010C9-1742-4B12-BEAF-A56E3EDBDF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098833E6-BDB1-462E-A5FA-453D508D4A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11170" xr2:uid="{D2F0FAED-A1B1-4AC7-BF59-91D91F5D52A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -500,7 +500,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1666,23 +1666,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D0D739-AE29-46AA-9B7E-F4AB12817690}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="51.5546875" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.90625" customWidth="1"/>
+    <col min="3" max="3" width="51.54296875" customWidth="1"/>
+    <col min="4" max="4" width="38.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
@@ -1778,7 +1778,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>57</v>
       </c>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1959,13 +1959,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>48</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>47</v>
       </c>

</xml_diff>